<commit_message>
Bug corrections/ addition of try/except blocks/ instructions form
</commit_message>
<xml_diff>
--- a/data/input/test.xlsx
+++ b/data/input/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisareade/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Desktop/DEVELOPMENT/FREELANCER/excelWeb_script/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9153659-F8EF-EB4F-8957-0DB1BB08E4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C765F1-328B-8546-B60A-8F0F1F0ACE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="740" windowWidth="17120" windowHeight="16660" xr2:uid="{23558508-D378-784D-89A8-EC3EDA2AD5C2}"/>
+    <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{23558508-D378-784D-89A8-EC3EDA2AD5C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1222,5 +1222,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>